<commit_message>
Dataset and Note changes
</commit_message>
<xml_diff>
--- a/January 2023 Analysis/New Analysis/sampleset/LibraryManagement_authentic_sampleset_no_space.xlsx
+++ b/January 2023 Analysis/New Analysis/sampleset/LibraryManagement_authentic_sampleset_no_space.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rashedhasan/Desktop/UNL/Research/Object relational mapping/Step 5 - Abstraction/OM-Solution_Mapping/OM-ML_Research/January 2023 Analysis/New Analysis/sampleset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747F67EB-1843-A941-AE84-9F8AD97736D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896E4383-6B8B-9145-A867-3F61A7FC70BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1400" windowWidth="28040" windowHeight="16380" xr2:uid="{9E606C90-6937-7643-AC22-ADE071A6A0E2}"/>
   </bookViews>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE80F2C-09A0-644A-8168-23135C5417CA}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>